<commit_message>
corrected error in file path missing underscore
</commit_message>
<xml_diff>
--- a/input/images/hospitalnotification/pdf/doc_version_overview.xlsx
+++ b/input/images/hospitalnotification/pdf/doc_version_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/SandBox/dk-medcom/input/images/hospitalnotification/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA0C508-FA47-C04E-B4D4-D762143E9534}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C066728-888E-B049-BDC3-1267861B43D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20560" yWindow="4160" windowWidth="26440" windowHeight="15440" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
   </bookViews>
@@ -111,16 +111,16 @@
     <t>t:/Igangværende opgaver/Moderniseret sygehusadvis/Standard_dokumentation/Release 1.0 FHIR advis/Overview_advis codes_HL7_FHIR_1.0.docx</t>
   </si>
   <si>
-    <t>Overview_advis codes_HL7_FHIR.pdf</t>
-  </si>
-  <si>
-    <t>https://github.com/hl7dk/dk-medcom/blob/master/input/images/hospitalnotification/pdf/Overview_advis codes_HL7_FHIR.pdf</t>
-  </si>
-  <si>
     <t>Oversigt_adviskoder_HL7_FHIR_1.0.docx</t>
   </si>
   <si>
     <t>t:/Igangværende opgaver/Moderniseret sygehusadvis/Standard_dokumentation/Release 1.0 FHIR advis/Oversigt_adviskoder_HL7_FHIR_1.0.docx</t>
+  </si>
+  <si>
+    <t>Overview_advis_codes_HL7_FHIR.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/hl7dk/dk-medcom/blob/master/input/images/hospitalnotification/pdf/Overview_advis_codes_HL7_FHIR.pdf</t>
   </si>
 </sst>
 </file>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79F97E6-EACE-4143-93BD-6BDF6CD549D5}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,13 +603,13 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1">
         <v>44224</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -629,7 +629,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Files for HospitalNotification updated and valueset updated with deceased
</commit_message>
<xml_diff>
--- a/input/images/hospitalnotification/pdf/doc_version_overview.xlsx
+++ b/input/images/hospitalnotification/pdf/doc_version_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/SandBox/dk-medcom/input/images/hospitalnotification/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C066728-888E-B049-BDC3-1267861B43D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BCF7BD-08B4-E646-B360-A0970F532DC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20560" yWindow="4160" windowWidth="26440" windowHeight="15440" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
+    <workbookView xWindow="20560" yWindow="11420" windowWidth="26440" windowHeight="15440" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
   </bookViews>
   <sheets>
     <sheet name="hospitalnotification" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,7 +538,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1">
-        <v>44223</v>
+        <v>44224</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -555,7 +555,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="1">
-        <v>44223</v>
+        <v>44224</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
use case documentation updated, copy paste error
</commit_message>
<xml_diff>
--- a/input/images/hospitalnotification/pdf/doc_version_overview.xlsx
+++ b/input/images/hospitalnotification/pdf/doc_version_overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/SandBox/dk-medcom/input/images/hospitalnotification/pdf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/SandBox/breaking/input/images/hospitalnotification/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BCF7BD-08B4-E646-B360-A0970F532DC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFBE44D-D290-BE44-BB4E-371F252EDEDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20560" yWindow="11420" windowWidth="26440" windowHeight="15440" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
+    <workbookView xWindow="22420" yWindow="4300" windowWidth="26440" windowHeight="15440" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
   </bookViews>
   <sheets>
     <sheet name="hospitalnotification" sheetId="1" r:id="rId1"/>
@@ -78,18 +78,6 @@
     <t>t:/Igangværende opgaver/Moderniseret sygehusadvis/Standard_dokumentation/Release 1.0 FHIR advis/FHIR_advis_om_sygehusophold_1.0.docx</t>
   </si>
   <si>
-    <t>Use_cases_advis_om_sygehusophold_vers1.0_260121.docx</t>
-  </si>
-  <si>
-    <t>t:/Igangværende opgaver/Moderniseret sygehusadvis/Standard_dokumentation/Release 1.0 FHIR advis/Use_cases_advis_om_sygehusophold_vers1.0_260121.docx</t>
-  </si>
-  <si>
-    <t>Use_cases_hospital_notification_vers1.0_260121.docx</t>
-  </si>
-  <si>
-    <t>t:/Igangværende opgaver/Moderniseret sygehusadvis/Standard_dokumentation/Release 1.0 FHIR advis/Use_cases_hospital_notification_vers1.0_260121.docx</t>
-  </si>
-  <si>
     <t>https://github.com/hl7dk/dk-medcom/blob/master/input/images/hospitalnotification/pdf/FHIR_Hospital_Notification.pdf</t>
   </si>
   <si>
@@ -121,6 +109,18 @@
   </si>
   <si>
     <t>https://github.com/hl7dk/dk-medcom/blob/master/input/images/hospitalnotification/pdf/Overview_advis_codes_HL7_FHIR.pdf</t>
+  </si>
+  <si>
+    <t>Use_cases_advis_om_sygehusophold_vers1.0.1_030221.docx</t>
+  </si>
+  <si>
+    <t>Use_cases_hospital_notification_vers1.0.1_030221.docx</t>
+  </si>
+  <si>
+    <t>t:/Igangværende opgaver/Moderniseret sygehusadvis/Standard_dokumentation/Release 1.0 FHIR advis/Use_cases_hospital_notification_vers1.0.1_030221.docx</t>
+  </si>
+  <si>
+    <t>t:/Igangværende opgaver/Moderniseret sygehusadvis/Standard_dokumentation/Release 1.0 FHIR advis/Use_cases_advis_om_sygehusophold_vers1.0.1_030221.docx</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,7 +561,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -569,16 +569,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1">
-        <v>44223</v>
+        <v>44232</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -586,50 +586,50 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1">
-        <v>44223</v>
+        <v>44232</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1">
         <v>44224</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
         <v>44224</v>
       </c>
       <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed column from advis codes
</commit_message>
<xml_diff>
--- a/input/images/hospitalnotification/pdf/doc_version_overview.xlsx
+++ b/input/images/hospitalnotification/pdf/doc_version_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/SandBox/breaking/input/images/hospitalnotification/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFBE44D-D290-BE44-BB4E-371F252EDEDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFD128B-D211-1E46-A3BF-3BEF0504EBD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22420" yWindow="4300" windowWidth="26440" windowHeight="15440" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
+    <workbookView xWindow="26400" yWindow="3520" windowWidth="40340" windowHeight="18280" xr2:uid="{F06FC630-43D2-7446-A1CF-075B49DE8C21}"/>
   </bookViews>
   <sheets>
     <sheet name="hospitalnotification" sheetId="1" r:id="rId1"/>
@@ -87,24 +87,12 @@
     <t>https://github.com/hl7dk/dk-medcom/blob/master/input/images/hospitalnotification/pdf/Use_cases_advis_om_sygehusophold.pdf</t>
   </si>
   <si>
-    <t>Overview_advis codes_HL7_FHIR_1.0.docx</t>
-  </si>
-  <si>
     <t>https://github.com/hl7dk/dk-medcom/blob/master/input/images/hospitalnotification/pdf/Oversigt_adviskoder_HL7_FHIR.pdf</t>
   </si>
   <si>
     <t>Oversigt_adviskoder_HL7_FHIR.pdf</t>
   </si>
   <si>
-    <t>t:/Igangværende opgaver/Moderniseret sygehusadvis/Standard_dokumentation/Release 1.0 FHIR advis/Overview_advis codes_HL7_FHIR_1.0.docx</t>
-  </si>
-  <si>
-    <t>Oversigt_adviskoder_HL7_FHIR_1.0.docx</t>
-  </si>
-  <si>
-    <t>t:/Igangværende opgaver/Moderniseret sygehusadvis/Standard_dokumentation/Release 1.0 FHIR advis/Oversigt_adviskoder_HL7_FHIR_1.0.docx</t>
-  </si>
-  <si>
     <t>Overview_advis_codes_HL7_FHIR.pdf</t>
   </si>
   <si>
@@ -121,6 +109,18 @@
   </si>
   <si>
     <t>t:/Igangværende opgaver/Moderniseret sygehusadvis/Standard_dokumentation/Release 1.0 FHIR advis/Use_cases_advis_om_sygehusophold_vers1.0.1_030221.docx</t>
+  </si>
+  <si>
+    <t>Oversigt_adviskoder_HL7_FHIR_1.0.1.doc</t>
+  </si>
+  <si>
+    <t>Overview_advis codes_HL7_FHIR_1.0.1.docx</t>
+  </si>
+  <si>
+    <t>https://teams.microsoft.com/l/file/731C0EC3-5C21-45F2-B54A-8F8D5CB1D510?tenantId=4898802a-6a02-437e-beb6-47cb8db2f43d&amp;fileType=docx&amp;objectUrl=https%3A%2F%2Fmedcomtest.sharepoint.com%2Fsites%2FFHIR-ModerniseringafMedComStandarder%2FDelte%20dokumenter%2FAdvis%20om%20sygehusophold%2FOversigt_adviskoder_HL7_FHIR_1.0.1.docx&amp;baseUrl=https%3A%2F%2Fmedcomtest.sharepoint.com%2Fsites%2FFHIR-ModerniseringafMedComStandarder&amp;serviceName=teams&amp;threadId=19:9f589d52d6f34e96ba534075c28d0abc@thread.skype&amp;groupId=6beb4dc7-667a-48c8-9716-18976d8b8329</t>
+  </si>
+  <si>
+    <t>https://teams.microsoft.com/l/file/B5D7D898-5663-45C6-9D91-D8A602BBA5FA?tenantId=4898802a-6a02-437e-beb6-47cb8db2f43d&amp;fileType=docx&amp;objectUrl=https%3A%2F%2Fmedcomtest.sharepoint.com%2Fsites%2FFHIR-ModerniseringafMedComStandarder%2FDelte%20dokumenter%2FAdvis%20om%20sygehusophold%2FOverview_advis%20codes_HL7_FHIR_1.0.1.docx&amp;baseUrl=https%3A%2F%2Fmedcomtest.sharepoint.com%2Fsites%2FFHIR-ModerniseringafMedComStandarder&amp;serviceName=teams&amp;threadId=19:9f589d52d6f34e96ba534075c28d0abc@thread.skype&amp;groupId=6beb4dc7-667a-48c8-9716-18976d8b8329</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,13 +569,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1">
         <v>44232</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -586,13 +586,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1">
         <v>44232</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -600,36 +600,36 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1">
         <v>44224</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1">
         <v>44224</v>
       </c>
       <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>